<commit_message>
Nuevo Template1.xlsx y mejoras informes
</commit_message>
<xml_diff>
--- a/appwebFAP/src/main/resources/Template1.xlsx
+++ b/appwebFAP/src/main/resources/Template1.xlsx
@@ -1,35 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B811D18-62A9-4E8D-AF76-01A361FCCA52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>customid</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>snbfh shgsgfsgfhsg dhfgsh dgj gsh gfjsdgfj 1</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -38,31 +25,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -77,17 +51,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -106,7 +72,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -181,6 +147,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -216,6 +199,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -391,48 +391,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.26953125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="61.81640625" style="4" customWidth="1"/>
-    <col min="3" max="16384" width="8.7265625" style="4"/>
+    <col min="1" max="1" width="12.26953125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7265625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7265625" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.26953125" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="26.81640625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.7265625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.7265625" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="8.7265625" style="1"/>
+    <col min="9" max="16384" width="8.7265625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1">
         <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="5">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.27559055118110237" right="0.27559055118110237" top="1.1417322834645669" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" fitToHeight="999" orientation="landscape" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;L&amp;G&amp;C&amp;"-,Negrita"&amp;14ACTA COMPETICION&amp;R&amp;D</oddHeader>
-    <oddFooter>&amp;CPágina &amp;P de &amp;N</oddFooter>
+    <oddHeader>&amp;L&amp;G&amp;C&amp;"Century Gothic,Negrita"&amp;12
+&amp;14Título&amp;R&amp;"Century Gothic,Negrita"&amp;10
+FEDERACIÓN ANDALUZA DE PATINAJE
+Comité Andaluz de Patinaje Freestyle
+&amp;9e-mail: &amp;K07+000comitefreestyle@fapatinaje.org</oddHeader>
+    <oddFooter>&amp;C&amp;"Century Gothic,Normal"&amp;10En Sevilla, a &amp;D&amp;R&amp;"Century Gothic,Negrita"&amp;10Fdo: José Antonio García
+Presidente Comité Andaluz de Patinaje Freestyle</oddFooter>
   </headerFooter>
   <legacyDrawingHF r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
Classic puntuaciones por juez
</commit_message>
<xml_diff>
--- a/appwebFAP/src/main/resources/Template1.xlsx
+++ b/appwebFAP/src/main/resources/Template1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B811D18-62A9-4E8D-AF76-01A361FCCA52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0FA1DCC-6DD8-4A22-900A-F4128C30D925}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -427,10 +427,10 @@
     <oddHeader>&amp;L&amp;G&amp;C&amp;"Century Gothic,Negrita"&amp;12
 &amp;14Título&amp;R&amp;"Century Gothic,Negrita"&amp;10
 FEDERACIÓN ANDALUZA DE PATINAJE
-Comité Andaluz de Patinaje Freestyle
+Comité Andaluz de Patinaje Inline Freestyle
 &amp;9e-mail: &amp;K07+000comitefreestyle@fapatinaje.org</oddHeader>
     <oddFooter>&amp;C&amp;"Century Gothic,Normal"&amp;10En Sevilla, a &amp;D&amp;R&amp;"Century Gothic,Negrita"&amp;10Fdo: José Antonio García
-Presidente Comité Andaluz de Patinaje Freestyle</oddFooter>
+Presidente Comité Andaluz de Patinaje Inline Freestyle</oddFooter>
   </headerFooter>
   <legacyDrawingHF r:id="rId2"/>
 </worksheet>

</xml_diff>